<commit_message>
AG Version: Fitness Failing finding solution
</commit_message>
<xml_diff>
--- a/Proyecto/data/horarioEstudiantes.xlsx
+++ b/Proyecto/data/horarioEstudiantes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Año</t>
   </si>
@@ -59,79 +59,73 @@
     <t>10IE2016</t>
   </si>
   <si>
+    <t>Profesor5segundoN5_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>Receso</t>
+  </si>
+  <si>
+    <t>Periodo Prohibido</t>
+  </si>
+  <si>
+    <t>Periodo Error: Cruzado</t>
+  </si>
+  <si>
+    <t>Periodo Libre</t>
+  </si>
+  <si>
+    <t>20IE2009</t>
+  </si>
+  <si>
+    <t>10IE2008</t>
+  </si>
+  <si>
+    <t>20IE2010</t>
+  </si>
+  <si>
+    <t>10IE2011</t>
+  </si>
+  <si>
+    <t>10IE2010</t>
+  </si>
+  <si>
+    <t>30IE2010</t>
+  </si>
+  <si>
+    <t>Profesor4SegundoN_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>30IE2009</t>
+  </si>
+  <si>
+    <t>30IE2010, 10IE2010</t>
+  </si>
+  <si>
+    <t>10IE2009</t>
+  </si>
+  <si>
     <t>DiegoPablo_RegaladoSamayoa</t>
   </si>
   <si>
-    <t>Receso</t>
-  </si>
-  <si>
-    <t>Periodo Prohibido</t>
-  </si>
-  <si>
-    <t>Periodo Error: Cruzado</t>
-  </si>
-  <si>
-    <t>Periodo Libre</t>
-  </si>
-  <si>
-    <t>10IE2010</t>
-  </si>
-  <si>
-    <t>20IE2010</t>
-  </si>
-  <si>
-    <t>20IE2009</t>
-  </si>
-  <si>
-    <t>Profesor4SegundoN_Apellido1Apellido2</t>
-  </si>
-  <si>
-    <t>10IE2011</t>
-  </si>
-  <si>
-    <t>30IE2010</t>
+    <t>20IE2010, 20IE2009</t>
+  </si>
+  <si>
+    <t>10IE2013</t>
+  </si>
+  <si>
+    <t>10IE3028</t>
+  </si>
+  <si>
+    <t>10IE3048</t>
+  </si>
+  <si>
+    <t>10IE3049</t>
   </si>
   <si>
     <t>Miguelnose_apellidoapellido2</t>
   </si>
   <si>
-    <t>MaurucioRodrigo_Apellido1Sepa</t>
-  </si>
-  <si>
-    <t>30IE2009</t>
-  </si>
-  <si>
-    <t>10IE2008, 10IE2009</t>
-  </si>
-  <si>
-    <t>10IE2008</t>
-  </si>
-  <si>
-    <t>10IE2009</t>
-  </si>
-  <si>
-    <t>Profesor5segundoN5_Apellido1Apellido2</t>
-  </si>
-  <si>
-    <t>30IE2010, 10IE2009</t>
-  </si>
-  <si>
-    <t>10IE3028</t>
-  </si>
-  <si>
-    <t>10IE3048</t>
-  </si>
-  <si>
-    <t>10IE2013</t>
-  </si>
-  <si>
-    <t>10IE3049</t>
-  </si>
-  <si>
     <t>20IE3028</t>
-  </si>
-  <si>
-    <t>10IE3048, 10IE2013</t>
   </si>
 </sst>
 </file>
@@ -812,9 +806,9 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="28" r="D5" t="s"/>
-      <c s="28" r="E5" t="s"/>
-      <c s="28" r="F5" t="s"/>
+      <c s="40" r="D5" t="s"/>
+      <c s="40" r="E5" t="s"/>
+      <c s="40" r="F5" t="s"/>
       <c s="28" r="G5" t="s"/>
       <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
@@ -837,9 +831,9 @@
         <v>0.3576388888888889</v>
       </c>
       <c s="28" r="D6" t="s"/>
-      <c s="28" r="E6" t="s"/>
-      <c s="31" r="F6" t="s"/>
-      <c s="32" r="G6" t="s"/>
+      <c s="40" r="E6" t="s"/>
+      <c s="40" r="F6" t="s"/>
+      <c s="40" r="G6" t="s"/>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
       <c s="30" r="J6" t="s"/>
@@ -857,8 +851,8 @@
         <v>0.3923611111111111</v>
       </c>
       <c s="28" r="D7" t="s"/>
-      <c s="33" r="E7" t="s"/>
-      <c s="34" r="F7" t="s"/>
+      <c s="40" r="E7" t="s"/>
+      <c s="40" r="F7" t="s"/>
       <c s="35" r="G7" t="s"/>
       <c s="36" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
@@ -876,10 +870,10 @@
       <c s="2" r="C8" t="n">
         <v>0.4270833333333333</v>
       </c>
-      <c s="28" r="D8" t="s"/>
-      <c s="28" r="E8" t="s"/>
-      <c s="36" r="F8" t="s"/>
-      <c s="28" r="G8" t="s"/>
+      <c s="40" r="D8" t="s"/>
+      <c s="40" r="E8" t="s"/>
+      <c s="40" r="F8" t="s"/>
+      <c s="40" r="G8" t="s"/>
       <c s="37" r="H8" t="s"/>
       <c s="29" r="I8" t="s"/>
       <c s="30" r="J8" t="s"/>
@@ -917,10 +911,12 @@
         <v>0.4756944444444444</v>
       </c>
       <c s="37" r="D10" t="s"/>
-      <c s="37" r="E10" t="s"/>
-      <c s="37" r="F10" t="s"/>
-      <c s="37" r="G10" t="s"/>
-      <c s="33" r="H10" t="s"/>
+      <c s="40" r="E10" t="s"/>
+      <c s="40" r="F10" t="s"/>
+      <c s="40" r="G10" t="s"/>
+      <c s="40" r="H10" t="s">
+        <v>12</v>
+      </c>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
       <c s="29" r="K10" t="s"/>
@@ -937,10 +933,10 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="32" r="D11" t="s"/>
-      <c s="28" r="E11" t="s"/>
+      <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
-      <c s="28" r="G11" t="s"/>
-      <c s="33" r="H11" t="s"/>
+      <c s="40" r="G11" t="s"/>
+      <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
       <c s="30" r="J11" t="s"/>
       <c s="29" r="K11" t="s"/>
@@ -957,10 +953,10 @@
         <v>0.5451388888888888</v>
       </c>
       <c s="28" r="D12" t="s"/>
-      <c s="28" r="E12" t="s"/>
-      <c s="32" r="F12" t="s"/>
+      <c s="40" r="E12" t="s"/>
+      <c s="40" r="F12" t="s"/>
       <c s="32" r="G12" t="s"/>
-      <c s="32" r="H12" t="s"/>
+      <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
       <c s="29" r="K12" t="s"/>
@@ -976,9 +972,9 @@
       <c s="2" r="C13" t="n">
         <v>0.5798611111111112</v>
       </c>
-      <c s="28" r="D13" t="s"/>
+      <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
-      <c s="28" r="F13" t="s"/>
+      <c s="40" r="F13" t="s"/>
       <c s="33" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
@@ -996,9 +992,9 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="28" r="D14" t="s"/>
-      <c s="28" r="E14" t="s"/>
-      <c s="28" r="F14" t="s"/>
+      <c s="40" r="D14" t="s"/>
+      <c s="40" r="E14" t="s"/>
+      <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
       <c s="28" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
@@ -1016,13 +1012,11 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="39" r="D15" t="s"/>
+      <c s="40" r="D15" t="s"/>
       <c s="33" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
-      <c s="40" r="H15" t="s">
-        <v>12</v>
-      </c>
+      <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -1038,11 +1032,11 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="32" r="D16" t="s"/>
+      <c s="40" r="D16" t="s"/>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
-      <c s="37" r="G16" t="s"/>
-      <c s="28" r="H16" t="s"/>
+      <c s="40" r="G16" t="s"/>
+      <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -1058,11 +1052,13 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="35" r="D17" t="s"/>
+      <c s="40" r="D17" t="s"/>
       <c s="28" r="E17" t="s"/>
-      <c s="28" r="F17" t="s"/>
+      <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="38" r="H17" t="s"/>
+      <c s="40" r="H17" t="s">
+        <v>12</v>
+      </c>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -1079,8 +1075,8 @@
         <v>0.7534722222222222</v>
       </c>
       <c s="28" r="D18" t="s"/>
-      <c s="36" r="E18" t="s"/>
-      <c s="35" r="F18" t="s"/>
+      <c s="40" r="E18" t="s"/>
+      <c s="40" r="F18" t="s"/>
       <c s="28" r="G18" t="s"/>
       <c s="32" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
@@ -1098,11 +1094,11 @@
       <c s="2" r="C19" t="n">
         <v>0.7881944444444444</v>
       </c>
-      <c s="38" r="D19" t="s"/>
+      <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
-      <c s="28" r="G19" t="s"/>
-      <c s="28" r="H19" t="s"/>
+      <c s="40" r="G19" t="s"/>
+      <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -1118,13 +1114,11 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="40" r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c s="32" r="E20" t="s"/>
-      <c s="28" r="F20" t="s"/>
+      <c s="40" r="D20" t="s"/>
+      <c s="40" r="E20" t="s"/>
+      <c s="40" r="F20" t="s"/>
       <c s="28" r="G20" t="s"/>
-      <c s="28" r="H20" t="s"/>
+      <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
       <c s="29" r="K20" t="s"/>
@@ -1140,13 +1134,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="28" r="D21" t="s"/>
-      <c s="40" r="E21" t="s">
-        <v>12</v>
-      </c>
+      <c s="40" r="D21" t="s"/>
+      <c s="40" r="E21" t="s"/>
       <c s="34" r="F21" t="s"/>
-      <c s="28" r="G21" t="s"/>
-      <c s="28" r="H21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -1166,7 +1158,9 @@
       <c s="41" r="E22" t="s"/>
       <c s="41" r="F22" t="s"/>
       <c s="41" r="G22" t="s"/>
-      <c s="41" r="H22" t="s"/>
+      <c s="41" r="H22" t="s">
+        <v>12</v>
+      </c>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -1292,15 +1286,17 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="28" r="D5" t="s"/>
-      <c s="28" r="E5" t="s"/>
-      <c s="41" r="F5" t="s">
+      <c s="40" r="D5" t="s">
         <v>18</v>
       </c>
-      <c s="28" r="G5" t="s"/>
+      <c s="40" r="E5" t="s"/>
+      <c s="41" r="F5" t="s"/>
+      <c s="40" r="G5" t="s">
+        <v>19</v>
+      </c>
       <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="30" r="J5" t="s">
         <v>13</v>
@@ -1318,16 +1314,20 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="28" r="D6" t="s"/>
-      <c s="28" r="E6" t="s"/>
-      <c s="41" r="F6" t="s"/>
-      <c s="32" r="G6" t="s"/>
+      <c s="40" r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c s="40" r="E6" t="s"/>
+      <c s="41" r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c s="40" r="G6" t="s"/>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c s="30" r="J6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1342,12 +1342,10 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="40" r="D7" t="s">
+      <c s="28" r="D7" t="s"/>
+      <c s="40" r="E7" t="s"/>
+      <c s="41" r="F7" t="s">
         <v>19</v>
-      </c>
-      <c s="33" r="E7" t="s"/>
-      <c s="41" r="F7" t="s">
-        <v>22</v>
       </c>
       <c s="35" r="G7" t="s"/>
       <c s="36" r="H7" t="s"/>
@@ -1355,7 +1353,7 @@
         <v>23</v>
       </c>
       <c s="30" r="J7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c s="29" r="K7" t="s"/>
       <c s="30" r="L7" t="s"/>
@@ -1370,16 +1368,20 @@
       <c s="2" r="C8" t="n">
         <v>0.4270833333333333</v>
       </c>
-      <c s="28" r="D8" t="s"/>
-      <c s="28" r="E8" t="s"/>
+      <c s="40" r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c s="40" r="E8" t="s"/>
       <c s="41" r="F8" t="s"/>
-      <c s="28" r="G8" t="s"/>
-      <c s="37" r="H8" t="s"/>
+      <c s="40" r="G8" t="s"/>
+      <c s="40" r="H8" t="s">
+        <v>20</v>
+      </c>
       <c s="29" r="I8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1400,10 +1402,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1418,20 +1420,22 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="37" r="D10" t="s"/>
-      <c s="37" r="E10" t="s"/>
+      <c s="40" r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c s="40" r="E10" t="s"/>
       <c s="41" r="F10" t="s"/>
       <c s="40" r="G10" t="s">
         <v>20</v>
       </c>
-      <c s="40" r="H10" t="s">
-        <v>18</v>
+      <c s="42" r="H10" t="s">
+        <v>26</v>
       </c>
       <c s="29" r="I10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c s="30" r="J10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c s="29" r="K10" t="s"/>
       <c s="30" r="L10" t="s"/>
@@ -1447,19 +1451,17 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="32" r="D11" t="s"/>
-      <c s="28" r="E11" t="s"/>
+      <c s="40" r="E11" t="s">
+        <v>23</v>
+      </c>
       <c s="41" r="F11" t="s"/>
-      <c s="40" r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c s="42" r="H11" t="s">
-        <v>27</v>
-      </c>
+      <c s="40" r="G11" t="s"/>
+      <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c s="30" r="J11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c s="29" r="K11" t="s"/>
       <c s="30" r="L11" t="s"/>
@@ -1475,17 +1477,15 @@
         <v>0.5451388888888888</v>
       </c>
       <c s="28" r="D12" t="s"/>
-      <c s="28" r="E12" t="s"/>
-      <c s="41" r="F12" t="s">
-        <v>26</v>
-      </c>
+      <c s="40" r="E12" t="s"/>
+      <c s="41" r="F12" t="s"/>
       <c s="32" r="G12" t="s"/>
-      <c s="32" r="H12" t="s"/>
+      <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c s="30" r="J12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c s="29" r="K12" t="s"/>
       <c s="30" r="L12" t="s"/>
@@ -1500,7 +1500,7 @@
       <c s="2" r="C13" t="n">
         <v>0.5798611111111112</v>
       </c>
-      <c s="28" r="D13" t="s"/>
+      <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
       <c s="41" r="F13" t="s"/>
       <c s="33" r="G13" t="s"/>
@@ -1520,14 +1520,12 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="28" r="D14" t="s"/>
-      <c s="42" r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c s="40" r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="D14" t="s"/>
+      <c s="40" r="E14" t="s"/>
+      <c s="40" r="F14" t="s"/>
+      <c s="40" r="G14" t="s">
+        <v>21</v>
+      </c>
       <c s="28" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -1544,11 +1542,15 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="39" r="D15" t="s"/>
+      <c s="40" r="D15" t="s"/>
       <c s="33" r="E15" t="s"/>
-      <c s="32" r="F15" t="s"/>
+      <c s="40" r="F15" t="s">
+        <v>22</v>
+      </c>
       <c s="28" r="G15" t="s"/>
-      <c s="28" r="H15" t="s"/>
+      <c s="40" r="H15" t="s">
+        <v>27</v>
+      </c>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -1564,13 +1566,13 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="32" r="D16" t="s"/>
+      <c s="40" r="D16" t="s"/>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
       <c s="40" r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c s="28" r="H16" t="s"/>
+        <v>25</v>
+      </c>
+      <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -1586,11 +1588,13 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="35" r="D17" t="s"/>
+      <c s="40" r="D17" t="s"/>
       <c s="28" r="E17" t="s"/>
-      <c s="28" r="F17" t="s"/>
+      <c s="42" r="F17" t="s">
+        <v>29</v>
+      </c>
       <c s="40" r="G17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c s="38" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
@@ -1609,12 +1613,12 @@
         <v>0.7534722222222222</v>
       </c>
       <c s="28" r="D18" t="s"/>
-      <c s="36" r="E18" t="s"/>
-      <c s="35" r="F18" t="s"/>
+      <c s="40" r="E18" t="s"/>
+      <c s="40" r="F18" t="s">
+        <v>27</v>
+      </c>
       <c s="28" r="G18" t="s"/>
-      <c s="40" r="H18" t="s">
-        <v>19</v>
-      </c>
+      <c s="32" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -1630,17 +1634,11 @@
       <c s="2" r="C19" t="n">
         <v>0.7881944444444444</v>
       </c>
-      <c s="40" r="D19" t="s">
-        <v>28</v>
-      </c>
+      <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
-      <c s="40" r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c s="40" r="G19" t="s">
-        <v>28</v>
-      </c>
-      <c s="28" r="H19" t="s"/>
+      <c s="28" r="F19" t="s"/>
+      <c s="40" r="G19" t="s"/>
+      <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -1656,15 +1654,11 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="28" r="D20" t="s"/>
-      <c s="40" r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c s="28" r="F20" t="s"/>
-      <c s="40" r="G20" t="s">
-        <v>23</v>
-      </c>
-      <c s="28" r="H20" t="s"/>
+      <c s="40" r="D20" t="s"/>
+      <c s="40" r="E20" t="s"/>
+      <c s="40" r="F20" t="s"/>
+      <c s="28" r="G20" t="s"/>
+      <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
       <c s="29" r="K20" t="s"/>
@@ -1680,11 +1674,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="28" r="D21" t="s"/>
-      <c s="28" r="E21" t="s"/>
+      <c s="40" r="D21" t="s"/>
+      <c s="40" r="E21" t="s"/>
       <c s="34" r="F21" t="s"/>
-      <c s="28" r="G21" t="s"/>
-      <c s="28" r="H21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -1700,11 +1694,11 @@
       <c s="2" r="C22" t="n">
         <v>0.8854166666666666</v>
       </c>
-      <c s="33" r="D22" t="s"/>
-      <c s="33" r="E22" t="s"/>
-      <c s="33" r="F22" t="s"/>
-      <c s="33" r="G22" t="s"/>
-      <c s="33" r="H22" t="s"/>
+      <c s="40" r="D22" t="s"/>
+      <c s="40" r="E22" t="s"/>
+      <c s="40" r="F22" t="s"/>
+      <c s="40" r="G22" t="s"/>
+      <c s="40" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -1829,13 +1823,15 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="28" r="D5" t="s"/>
-      <c s="28" r="E5" t="s"/>
-      <c s="28" r="F5" t="s"/>
-      <c s="41" r="G5" t="s"/>
+      <c s="40" r="D5" t="s"/>
+      <c s="40" r="E5" t="s"/>
+      <c s="40" r="F5" t="s"/>
+      <c s="41" r="G5" t="s">
+        <v>30</v>
+      </c>
       <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c s="30" r="J5" t="s">
         <v>24</v>
@@ -1854,15 +1850,17 @@
         <v>0.3576388888888889</v>
       </c>
       <c s="28" r="D6" t="s"/>
-      <c s="28" r="E6" t="s"/>
-      <c s="31" r="F6" t="s"/>
-      <c s="41" r="G6" t="s"/>
+      <c s="40" r="E6" t="s"/>
+      <c s="40" r="F6" t="s"/>
+      <c s="41" r="G6" t="s">
+        <v>30</v>
+      </c>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c s="30" r="J6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1878,15 +1876,15 @@
         <v>0.3923611111111111</v>
       </c>
       <c s="28" r="D7" t="s"/>
-      <c s="33" r="E7" t="s"/>
-      <c s="34" r="F7" t="s"/>
+      <c s="40" r="E7" t="s"/>
+      <c s="40" r="F7" t="s"/>
       <c s="41" r="G7" t="s"/>
       <c s="36" r="H7" t="s"/>
       <c s="29" r="I7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c s="30" r="J7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c s="29" r="K7" t="s"/>
       <c s="30" r="L7" t="s"/>
@@ -1901,16 +1899,16 @@
       <c s="2" r="C8" t="n">
         <v>0.4270833333333333</v>
       </c>
-      <c s="28" r="D8" t="s"/>
-      <c s="28" r="E8" t="s"/>
-      <c s="36" r="F8" t="s"/>
+      <c s="40" r="D8" t="s"/>
+      <c s="40" r="E8" t="s"/>
+      <c s="40" r="F8" t="s"/>
       <c s="41" r="G8" t="s"/>
       <c s="37" r="H8" t="s"/>
       <c s="29" r="I8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1931,10 +1929,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1950,14 +1948,10 @@
         <v>0.4756944444444444</v>
       </c>
       <c s="37" r="D10" t="s"/>
-      <c s="37" r="E10" t="s"/>
-      <c s="40" r="F10" t="s">
-        <v>35</v>
-      </c>
+      <c s="40" r="E10" t="s"/>
+      <c s="40" r="F10" t="s"/>
       <c s="41" r="G10" t="s"/>
-      <c s="40" r="H10" t="s">
-        <v>36</v>
-      </c>
+      <c s="33" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
       <c s="29" r="K10" t="s"/>
@@ -1973,13 +1967,17 @@
       <c s="2" r="C11" t="n">
         <v>0.5104166666666666</v>
       </c>
-      <c s="32" r="D11" t="s"/>
-      <c s="40" r="E11" t="s">
-        <v>32</v>
-      </c>
+      <c s="40" r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
-      <c s="41" r="G11" t="s"/>
-      <c s="33" r="H11" t="s"/>
+      <c s="41" r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c s="40" r="H11" t="s">
+        <v>30</v>
+      </c>
       <c s="29" r="I11" t="s"/>
       <c s="30" r="J11" t="s"/>
       <c s="29" r="K11" t="s"/>
@@ -1996,10 +1994,12 @@
         <v>0.5451388888888888</v>
       </c>
       <c s="28" r="D12" t="s"/>
-      <c s="28" r="E12" t="s"/>
-      <c s="32" r="F12" t="s"/>
+      <c s="40" r="E12" t="s"/>
+      <c s="40" r="F12" t="s">
+        <v>33</v>
+      </c>
       <c s="41" r="G12" t="s"/>
-      <c s="32" r="H12" t="s"/>
+      <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
       <c s="29" r="K12" t="s"/>
@@ -2015,9 +2015,11 @@
       <c s="2" r="C13" t="n">
         <v>0.5798611111111112</v>
       </c>
-      <c s="28" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
-      <c s="28" r="F13" t="s"/>
+      <c s="40" r="D13" t="s"/>
+      <c s="40" r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c s="40" r="F13" t="s"/>
       <c s="41" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
@@ -2035,13 +2037,11 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="28" r="D14" t="s"/>
-      <c s="28" r="E14" t="s"/>
-      <c s="28" r="F14" t="s"/>
+      <c s="40" r="D14" t="s"/>
+      <c s="40" r="E14" t="s"/>
+      <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
-      <c s="40" r="H14" t="s">
-        <v>32</v>
-      </c>
+      <c s="28" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -2057,11 +2057,11 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="39" r="D15" t="s"/>
+      <c s="40" r="D15" t="s"/>
       <c s="33" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
-      <c s="28" r="H15" t="s"/>
+      <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -2077,13 +2077,17 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="32" r="D16" t="s"/>
-      <c s="40" r="E16" t="s">
-        <v>34</v>
-      </c>
+      <c s="40" r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
-      <c s="37" r="G16" t="s"/>
-      <c s="28" r="H16" t="s"/>
+      <c s="40" r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c s="40" r="H16" t="s">
+        <v>33</v>
+      </c>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -2099,13 +2103,11 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="35" r="D17" t="s"/>
+      <c s="40" r="D17" t="s"/>
       <c s="28" r="E17" t="s"/>
-      <c s="28" r="F17" t="s"/>
+      <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="40" r="H17" t="s">
-        <v>35</v>
-      </c>
+      <c s="38" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -2121,11 +2123,9 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="40" r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c s="36" r="E18" t="s"/>
-      <c s="35" r="F18" t="s"/>
+      <c s="28" r="D18" t="s"/>
+      <c s="40" r="E18" t="s"/>
+      <c s="40" r="F18" t="s"/>
       <c s="28" r="G18" t="s"/>
       <c s="32" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
@@ -2143,11 +2143,13 @@
       <c s="2" r="C19" t="n">
         <v>0.7881944444444444</v>
       </c>
-      <c s="38" r="D19" t="s"/>
+      <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
-      <c s="28" r="G19" t="s"/>
-      <c s="28" r="H19" t="s"/>
+      <c s="40" r="G19" t="s"/>
+      <c s="40" r="H19" t="s">
+        <v>31</v>
+      </c>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -2163,13 +2165,11 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="28" r="D20" t="s"/>
-      <c s="32" r="E20" t="s"/>
-      <c s="28" r="F20" t="s"/>
+      <c s="40" r="D20" t="s"/>
+      <c s="40" r="E20" t="s"/>
+      <c s="40" r="F20" t="s"/>
       <c s="28" r="G20" t="s"/>
-      <c s="42" r="H20" t="s">
-        <v>37</v>
-      </c>
+      <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
       <c s="29" r="K20" t="s"/>
@@ -2185,15 +2185,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="28" r="D21" t="s"/>
-      <c s="40" r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c s="40" r="F21" t="s">
-        <v>36</v>
-      </c>
-      <c s="28" r="G21" t="s"/>
-      <c s="28" r="H21" t="s"/>
+      <c s="40" r="D21" t="s"/>
+      <c s="40" r="E21" t="s"/>
+      <c s="34" r="F21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -2209,11 +2205,11 @@
       <c s="2" r="C22" t="n">
         <v>0.8854166666666666</v>
       </c>
-      <c s="33" r="D22" t="s"/>
-      <c s="33" r="E22" t="s"/>
-      <c s="33" r="F22" t="s"/>
-      <c s="33" r="G22" t="s"/>
-      <c s="33" r="H22" t="s"/>
+      <c s="40" r="D22" t="s"/>
+      <c s="40" r="E22" t="s"/>
+      <c s="40" r="F22" t="s"/>
+      <c s="40" r="G22" t="s"/>
+      <c s="40" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -2338,9 +2334,9 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="28" r="D5" t="s"/>
-      <c s="28" r="E5" t="s"/>
-      <c s="28" r="F5" t="s"/>
+      <c s="40" r="D5" t="s"/>
+      <c s="40" r="E5" t="s"/>
+      <c s="40" r="F5" t="s"/>
       <c s="28" r="G5" t="s"/>
       <c s="41" r="H5" t="s"/>
       <c s="29" r="I5" t="s"/>
@@ -2359,9 +2355,9 @@
         <v>0.3576388888888889</v>
       </c>
       <c s="28" r="D6" t="s"/>
-      <c s="28" r="E6" t="s"/>
-      <c s="31" r="F6" t="s"/>
-      <c s="32" r="G6" t="s"/>
+      <c s="40" r="E6" t="s"/>
+      <c s="40" r="F6" t="s"/>
+      <c s="40" r="G6" t="s"/>
       <c s="41" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
       <c s="30" r="J6" t="s"/>
@@ -2379,8 +2375,8 @@
         <v>0.3923611111111111</v>
       </c>
       <c s="28" r="D7" t="s"/>
-      <c s="33" r="E7" t="s"/>
-      <c s="34" r="F7" t="s"/>
+      <c s="40" r="E7" t="s"/>
+      <c s="40" r="F7" t="s"/>
       <c s="35" r="G7" t="s"/>
       <c s="41" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
@@ -2398,10 +2394,10 @@
       <c s="2" r="C8" t="n">
         <v>0.4270833333333333</v>
       </c>
-      <c s="28" r="D8" t="s"/>
-      <c s="28" r="E8" t="s"/>
-      <c s="36" r="F8" t="s"/>
-      <c s="28" r="G8" t="s"/>
+      <c s="40" r="D8" t="s"/>
+      <c s="40" r="E8" t="s"/>
+      <c s="40" r="F8" t="s"/>
+      <c s="40" r="G8" t="s"/>
       <c s="41" r="H8" t="s"/>
       <c s="29" r="I8" t="s"/>
       <c s="30" r="J8" t="s"/>
@@ -2439,9 +2435,9 @@
         <v>0.4756944444444444</v>
       </c>
       <c s="37" r="D10" t="s"/>
-      <c s="37" r="E10" t="s"/>
-      <c s="37" r="F10" t="s"/>
-      <c s="37" r="G10" t="s"/>
+      <c s="40" r="E10" t="s"/>
+      <c s="40" r="F10" t="s"/>
+      <c s="40" r="G10" t="s"/>
       <c s="41" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
@@ -2459,9 +2455,9 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="32" r="D11" t="s"/>
-      <c s="28" r="E11" t="s"/>
+      <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
-      <c s="28" r="G11" t="s"/>
+      <c s="40" r="G11" t="s"/>
       <c s="41" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
       <c s="30" r="J11" t="s"/>
@@ -2479,8 +2475,8 @@
         <v>0.5451388888888888</v>
       </c>
       <c s="28" r="D12" t="s"/>
-      <c s="28" r="E12" t="s"/>
-      <c s="32" r="F12" t="s"/>
+      <c s="40" r="E12" t="s"/>
+      <c s="40" r="F12" t="s"/>
       <c s="32" r="G12" t="s"/>
       <c s="41" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
@@ -2498,9 +2494,9 @@
       <c s="2" r="C13" t="n">
         <v>0.5798611111111112</v>
       </c>
-      <c s="28" r="D13" t="s"/>
+      <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
-      <c s="28" r="F13" t="s"/>
+      <c s="40" r="F13" t="s"/>
       <c s="33" r="G13" t="s"/>
       <c s="41" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
@@ -2518,9 +2514,9 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="28" r="D14" t="s"/>
-      <c s="28" r="E14" t="s"/>
-      <c s="28" r="F14" t="s"/>
+      <c s="40" r="D14" t="s"/>
+      <c s="40" r="E14" t="s"/>
+      <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
       <c s="28" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
@@ -2538,11 +2534,11 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="39" r="D15" t="s"/>
+      <c s="40" r="D15" t="s"/>
       <c s="33" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
-      <c s="28" r="H15" t="s"/>
+      <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -2558,11 +2554,11 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="32" r="D16" t="s"/>
+      <c s="40" r="D16" t="s"/>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
-      <c s="37" r="G16" t="s"/>
-      <c s="28" r="H16" t="s"/>
+      <c s="40" r="G16" t="s"/>
+      <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -2578,9 +2574,9 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="35" r="D17" t="s"/>
+      <c s="40" r="D17" t="s"/>
       <c s="28" r="E17" t="s"/>
-      <c s="28" r="F17" t="s"/>
+      <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
       <c s="38" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
@@ -2599,8 +2595,8 @@
         <v>0.7534722222222222</v>
       </c>
       <c s="28" r="D18" t="s"/>
-      <c s="36" r="E18" t="s"/>
-      <c s="35" r="F18" t="s"/>
+      <c s="40" r="E18" t="s"/>
+      <c s="40" r="F18" t="s"/>
       <c s="28" r="G18" t="s"/>
       <c s="32" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
@@ -2618,11 +2614,11 @@
       <c s="2" r="C19" t="n">
         <v>0.7881944444444444</v>
       </c>
-      <c s="38" r="D19" t="s"/>
+      <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
-      <c s="28" r="G19" t="s"/>
-      <c s="28" r="H19" t="s"/>
+      <c s="40" r="G19" t="s"/>
+      <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -2638,11 +2634,11 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="28" r="D20" t="s"/>
-      <c s="32" r="E20" t="s"/>
-      <c s="28" r="F20" t="s"/>
+      <c s="40" r="D20" t="s"/>
+      <c s="40" r="E20" t="s"/>
+      <c s="40" r="F20" t="s"/>
       <c s="28" r="G20" t="s"/>
-      <c s="28" r="H20" t="s"/>
+      <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
       <c s="29" r="K20" t="s"/>
@@ -2658,11 +2654,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="28" r="D21" t="s"/>
-      <c s="28" r="E21" t="s"/>
+      <c s="40" r="D21" t="s"/>
+      <c s="40" r="E21" t="s"/>
       <c s="34" r="F21" t="s"/>
-      <c s="28" r="G21" t="s"/>
-      <c s="28" r="H21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -2678,11 +2674,11 @@
       <c s="2" r="C22" t="n">
         <v>0.8854166666666666</v>
       </c>
-      <c s="33" r="D22" t="s"/>
-      <c s="33" r="E22" t="s"/>
-      <c s="33" r="F22" t="s"/>
-      <c s="33" r="G22" t="s"/>
-      <c s="33" r="H22" t="s"/>
+      <c s="40" r="D22" t="s"/>
+      <c s="40" r="E22" t="s"/>
+      <c s="40" r="F22" t="s"/>
+      <c s="40" r="G22" t="s"/>
+      <c s="40" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -2808,8 +2804,8 @@
         <v>0.3229166666666667</v>
       </c>
       <c s="41" r="D5" t="s"/>
-      <c s="28" r="E5" t="s"/>
-      <c s="28" r="F5" t="s"/>
+      <c s="40" r="E5" t="s"/>
+      <c s="40" r="F5" t="s"/>
       <c s="28" r="G5" t="s"/>
       <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s"/>
@@ -2828,9 +2824,9 @@
         <v>0.3576388888888889</v>
       </c>
       <c s="41" r="D6" t="s"/>
-      <c s="28" r="E6" t="s"/>
-      <c s="31" r="F6" t="s"/>
-      <c s="32" r="G6" t="s"/>
+      <c s="40" r="E6" t="s"/>
+      <c s="40" r="F6" t="s"/>
+      <c s="40" r="G6" t="s"/>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
       <c s="30" r="J6" t="s"/>
@@ -2848,8 +2844,8 @@
         <v>0.3923611111111111</v>
       </c>
       <c s="41" r="D7" t="s"/>
-      <c s="33" r="E7" t="s"/>
-      <c s="34" r="F7" t="s"/>
+      <c s="40" r="E7" t="s"/>
+      <c s="40" r="F7" t="s"/>
       <c s="35" r="G7" t="s"/>
       <c s="36" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
@@ -2868,9 +2864,9 @@
         <v>0.4270833333333333</v>
       </c>
       <c s="41" r="D8" t="s"/>
-      <c s="28" r="E8" t="s"/>
-      <c s="36" r="F8" t="s"/>
-      <c s="28" r="G8" t="s"/>
+      <c s="40" r="E8" t="s"/>
+      <c s="40" r="F8" t="s"/>
+      <c s="40" r="G8" t="s"/>
       <c s="37" r="H8" t="s"/>
       <c s="29" r="I8" t="s"/>
       <c s="30" r="J8" t="s"/>
@@ -2908,9 +2904,9 @@
         <v>0.4756944444444444</v>
       </c>
       <c s="41" r="D10" t="s"/>
-      <c s="37" r="E10" t="s"/>
-      <c s="37" r="F10" t="s"/>
-      <c s="37" r="G10" t="s"/>
+      <c s="40" r="E10" t="s"/>
+      <c s="40" r="F10" t="s"/>
+      <c s="40" r="G10" t="s"/>
       <c s="33" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
@@ -2928,10 +2924,10 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="41" r="D11" t="s"/>
-      <c s="28" r="E11" t="s"/>
+      <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
-      <c s="28" r="G11" t="s"/>
-      <c s="33" r="H11" t="s"/>
+      <c s="40" r="G11" t="s"/>
+      <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
       <c s="30" r="J11" t="s"/>
       <c s="29" r="K11" t="s"/>
@@ -2948,10 +2944,10 @@
         <v>0.5451388888888888</v>
       </c>
       <c s="41" r="D12" t="s"/>
-      <c s="28" r="E12" t="s"/>
-      <c s="32" r="F12" t="s"/>
+      <c s="40" r="E12" t="s"/>
+      <c s="40" r="F12" t="s"/>
       <c s="32" r="G12" t="s"/>
-      <c s="32" r="H12" t="s"/>
+      <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
       <c s="29" r="K12" t="s"/>
@@ -2969,7 +2965,7 @@
       </c>
       <c s="41" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
-      <c s="28" r="F13" t="s"/>
+      <c s="40" r="F13" t="s"/>
       <c s="33" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
@@ -2987,9 +2983,9 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="28" r="D14" t="s"/>
-      <c s="28" r="E14" t="s"/>
-      <c s="28" r="F14" t="s"/>
+      <c s="40" r="D14" t="s"/>
+      <c s="40" r="E14" t="s"/>
+      <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
       <c s="28" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
@@ -3007,11 +3003,11 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="39" r="D15" t="s"/>
+      <c s="40" r="D15" t="s"/>
       <c s="33" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
-      <c s="28" r="H15" t="s"/>
+      <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -3027,11 +3023,11 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="32" r="D16" t="s"/>
+      <c s="40" r="D16" t="s"/>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
-      <c s="37" r="G16" t="s"/>
-      <c s="28" r="H16" t="s"/>
+      <c s="40" r="G16" t="s"/>
+      <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -3047,9 +3043,9 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="35" r="D17" t="s"/>
+      <c s="40" r="D17" t="s"/>
       <c s="28" r="E17" t="s"/>
-      <c s="28" r="F17" t="s"/>
+      <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
       <c s="38" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
@@ -3068,8 +3064,8 @@
         <v>0.7534722222222222</v>
       </c>
       <c s="28" r="D18" t="s"/>
-      <c s="36" r="E18" t="s"/>
-      <c s="35" r="F18" t="s"/>
+      <c s="40" r="E18" t="s"/>
+      <c s="40" r="F18" t="s"/>
       <c s="28" r="G18" t="s"/>
       <c s="32" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
@@ -3087,11 +3083,11 @@
       <c s="2" r="C19" t="n">
         <v>0.7881944444444444</v>
       </c>
-      <c s="38" r="D19" t="s"/>
+      <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
-      <c s="28" r="G19" t="s"/>
-      <c s="28" r="H19" t="s"/>
+      <c s="40" r="G19" t="s"/>
+      <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -3107,11 +3103,11 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="28" r="D20" t="s"/>
-      <c s="32" r="E20" t="s"/>
-      <c s="28" r="F20" t="s"/>
+      <c s="40" r="D20" t="s"/>
+      <c s="40" r="E20" t="s"/>
+      <c s="40" r="F20" t="s"/>
       <c s="28" r="G20" t="s"/>
-      <c s="28" r="H20" t="s"/>
+      <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
       <c s="29" r="K20" t="s"/>
@@ -3127,11 +3123,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="28" r="D21" t="s"/>
-      <c s="28" r="E21" t="s"/>
+      <c s="40" r="D21" t="s"/>
+      <c s="40" r="E21" t="s"/>
       <c s="34" r="F21" t="s"/>
-      <c s="28" r="G21" t="s"/>
-      <c s="28" r="H21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -3147,11 +3143,11 @@
       <c s="2" r="C22" t="n">
         <v>0.8854166666666666</v>
       </c>
-      <c s="33" r="D22" t="s"/>
-      <c s="33" r="E22" t="s"/>
-      <c s="33" r="F22" t="s"/>
-      <c s="33" r="G22" t="s"/>
-      <c s="33" r="H22" t="s"/>
+      <c s="40" r="D22" t="s"/>
+      <c s="40" r="E22" t="s"/>
+      <c s="40" r="F22" t="s"/>
+      <c s="40" r="G22" t="s"/>
+      <c s="40" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>

</xml_diff>

<commit_message>
AG working, need better fitness
</commit_message>
<xml_diff>
--- a/Proyecto/data/horarioEstudiantes.xlsx
+++ b/Proyecto/data/horarioEstudiantes.xlsx
@@ -59,73 +59,73 @@
     <t>10IE2016</t>
   </si>
   <si>
+    <t>DiegoPablo_RegaladoSamayoa</t>
+  </si>
+  <si>
+    <t>Receso</t>
+  </si>
+  <si>
+    <t>Periodo Prohibido</t>
+  </si>
+  <si>
+    <t>Periodo Error: Cruzado</t>
+  </si>
+  <si>
+    <t>Periodo Libre</t>
+  </si>
+  <si>
+    <t>30IE2010</t>
+  </si>
+  <si>
+    <t>30IE2009</t>
+  </si>
+  <si>
+    <t>10IE2008</t>
+  </si>
+  <si>
+    <t>20IE2010</t>
+  </si>
+  <si>
+    <t>Profesor4SegundoN_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>20IE2009</t>
+  </si>
+  <si>
     <t>Profesor5segundoN5_Apellido1Apellido2</t>
   </si>
   <si>
-    <t>Receso</t>
-  </si>
-  <si>
-    <t>Periodo Prohibido</t>
-  </si>
-  <si>
-    <t>Periodo Error: Cruzado</t>
-  </si>
-  <si>
-    <t>Periodo Libre</t>
-  </si>
-  <si>
-    <t>20IE2009</t>
-  </si>
-  <si>
-    <t>10IE2008</t>
-  </si>
-  <si>
-    <t>20IE2010</t>
+    <t>10IE2010</t>
   </si>
   <si>
     <t>10IE2011</t>
   </si>
   <si>
-    <t>10IE2010</t>
-  </si>
-  <si>
-    <t>30IE2010</t>
-  </si>
-  <si>
-    <t>Profesor4SegundoN_Apellido1Apellido2</t>
-  </si>
-  <si>
-    <t>30IE2009</t>
-  </si>
-  <si>
-    <t>30IE2010, 10IE2010</t>
-  </si>
-  <si>
     <t>10IE2009</t>
   </si>
   <si>
-    <t>DiegoPablo_RegaladoSamayoa</t>
-  </si>
-  <si>
-    <t>20IE2010, 20IE2009</t>
+    <t>Miguelnose_apellidoapellido2</t>
+  </si>
+  <si>
+    <t>10IE3028</t>
+  </si>
+  <si>
+    <t>20IE3028</t>
+  </si>
+  <si>
+    <t>MaurucioRodrigo_Apellido1Sepa</t>
+  </si>
+  <si>
+    <t>10IE3028, 10IE3049, 20IE3028</t>
+  </si>
+  <si>
+    <t>10IE3048</t>
+  </si>
+  <si>
+    <t>10IE3049</t>
   </si>
   <si>
     <t>10IE2013</t>
-  </si>
-  <si>
-    <t>10IE3028</t>
-  </si>
-  <si>
-    <t>10IE3048</t>
-  </si>
-  <si>
-    <t>10IE3049</t>
-  </si>
-  <si>
-    <t>Miguelnose_apellidoapellido2</t>
-  </si>
-  <si>
-    <t>20IE3028</t>
   </si>
 </sst>
 </file>
@@ -810,7 +810,9 @@
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
       <c s="28" r="G5" t="s"/>
-      <c s="28" r="H5" t="s"/>
+      <c s="40" r="H5" t="s">
+        <v>12</v>
+      </c>
       <c s="29" r="I5" t="s">
         <v>12</v>
       </c>
@@ -832,7 +834,9 @@
       </c>
       <c s="28" r="D6" t="s"/>
       <c s="40" r="E6" t="s"/>
-      <c s="40" r="F6" t="s"/>
+      <c s="40" r="F6" t="s">
+        <v>12</v>
+      </c>
       <c s="40" r="G6" t="s"/>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
@@ -852,9 +856,11 @@
       </c>
       <c s="28" r="D7" t="s"/>
       <c s="40" r="E7" t="s"/>
-      <c s="40" r="F7" t="s"/>
+      <c s="40" r="F7" t="s">
+        <v>12</v>
+      </c>
       <c s="35" r="G7" t="s"/>
-      <c s="36" r="H7" t="s"/>
+      <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
       <c s="30" r="J7" t="s"/>
       <c s="29" r="K7" t="s"/>
@@ -914,9 +920,7 @@
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="40" r="G10" t="s"/>
-      <c s="40" r="H10" t="s">
-        <v>12</v>
-      </c>
+      <c s="40" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
       <c s="29" r="K10" t="s"/>
@@ -932,7 +936,7 @@
       <c s="2" r="C11" t="n">
         <v>0.5104166666666666</v>
       </c>
-      <c s="32" r="D11" t="s"/>
+      <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
@@ -975,7 +979,7 @@
       <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
-      <c s="33" r="G13" t="s"/>
+      <c s="40" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
@@ -996,7 +1000,7 @@
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
-      <c s="28" r="H14" t="s"/>
+      <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -1013,7 +1017,7 @@
         <v>0.6493055555555556</v>
       </c>
       <c s="40" r="D15" t="s"/>
-      <c s="33" r="E15" t="s"/>
+      <c s="40" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
@@ -1056,9 +1060,7 @@
       <c s="28" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="40" r="H17" t="s">
-        <v>12</v>
-      </c>
+      <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -1117,7 +1119,7 @@
       <c s="40" r="D20" t="s"/>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
-      <c s="28" r="G20" t="s"/>
+      <c s="40" r="G20" t="s"/>
       <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
@@ -1158,9 +1160,7 @@
       <c s="41" r="E22" t="s"/>
       <c s="41" r="F22" t="s"/>
       <c s="41" r="G22" t="s"/>
-      <c s="41" r="H22" t="s">
-        <v>12</v>
-      </c>
+      <c s="41" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -1289,17 +1289,19 @@
       <c s="40" r="D5" t="s">
         <v>18</v>
       </c>
-      <c s="40" r="E5" t="s"/>
+      <c s="40" r="E5" t="s">
+        <v>19</v>
+      </c>
       <c s="41" r="F5" t="s"/>
       <c s="40" r="G5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="30" r="J5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c s="29" r="K5" t="s"/>
       <c s="30" r="L5" t="s"/>
@@ -1315,19 +1317,21 @@
         <v>0.3576388888888889</v>
       </c>
       <c s="40" r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c s="40" r="E6" t="s"/>
-      <c s="41" r="F6" t="s">
+      <c s="41" r="F6" t="s"/>
+      <c s="40" r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c s="40" r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c s="29" r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c s="30" r="J6" t="s">
         <v>22</v>
-      </c>
-      <c s="40" r="G6" t="s"/>
-      <c s="31" r="H6" t="s"/>
-      <c s="29" r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c s="30" r="J6" t="s">
-        <v>13</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1342,15 +1346,17 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="28" r="D7" t="s"/>
+      <c s="40" r="D7" t="s">
+        <v>18</v>
+      </c>
       <c s="40" r="E7" t="s"/>
-      <c s="41" r="F7" t="s">
-        <v>19</v>
-      </c>
+      <c s="41" r="F7" t="s"/>
       <c s="35" r="G7" t="s"/>
-      <c s="36" r="H7" t="s"/>
+      <c s="40" r="H7" t="s">
+        <v>20</v>
+      </c>
       <c s="29" r="I7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c s="30" r="J7" t="s">
         <v>24</v>
@@ -1368,20 +1374,18 @@
       <c s="2" r="C8" t="n">
         <v>0.4270833333333333</v>
       </c>
-      <c s="40" r="D8" t="s">
-        <v>25</v>
-      </c>
+      <c s="40" r="D8" t="s"/>
       <c s="40" r="E8" t="s"/>
       <c s="41" r="F8" t="s"/>
       <c s="40" r="G8" t="s"/>
       <c s="40" r="H8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c s="29" r="I8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1402,10 +1406,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1420,22 +1424,20 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="40" r="D10" t="s">
+      <c s="37" r="D10" t="s"/>
+      <c s="40" r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c s="41" r="F10" t="s"/>
+      <c s="40" r="G10" t="s"/>
+      <c s="40" r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c s="29" r="I10" t="s">
         <v>19</v>
       </c>
-      <c s="40" r="E10" t="s"/>
-      <c s="41" r="F10" t="s"/>
-      <c s="40" r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c s="42" r="H10" t="s">
-        <v>26</v>
-      </c>
-      <c s="29" r="I10" t="s">
-        <v>25</v>
-      </c>
       <c s="30" r="J10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c s="29" r="K10" t="s"/>
       <c s="30" r="L10" t="s"/>
@@ -1450,15 +1452,15 @@
       <c s="2" r="C11" t="n">
         <v>0.5104166666666666</v>
       </c>
-      <c s="32" r="D11" t="s"/>
+      <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c s="41" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
       <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="30" r="J11" t="s">
         <v>13</v>
@@ -1503,7 +1505,7 @@
       <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
       <c s="41" r="F13" t="s"/>
-      <c s="33" r="G13" t="s"/>
+      <c s="40" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
@@ -1523,10 +1525,8 @@
       <c s="40" r="D14" t="s"/>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="40" r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c s="28" r="H14" t="s"/>
+      <c s="32" r="G14" t="s"/>
+      <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -1543,14 +1543,12 @@
         <v>0.6493055555555556</v>
       </c>
       <c s="40" r="D15" t="s"/>
-      <c s="33" r="E15" t="s"/>
-      <c s="40" r="F15" t="s">
-        <v>22</v>
-      </c>
+      <c s="40" r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
-      <c s="40" r="H15" t="s">
-        <v>27</v>
-      </c>
+      <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -1566,11 +1564,13 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="40" r="D16" t="s"/>
+      <c s="40" r="D16" t="s">
+        <v>26</v>
+      </c>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
       <c s="40" r="G16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
@@ -1588,15 +1588,13 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="40" r="D17" t="s"/>
+      <c s="40" r="D17" t="s">
+        <v>26</v>
+      </c>
       <c s="28" r="E17" t="s"/>
-      <c s="42" r="F17" t="s">
-        <v>29</v>
-      </c>
-      <c s="40" r="G17" t="s">
-        <v>23</v>
-      </c>
-      <c s="38" r="H17" t="s"/>
+      <c s="40" r="F17" t="s"/>
+      <c s="28" r="G17" t="s"/>
+      <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -1614,11 +1612,11 @@
       </c>
       <c s="28" r="D18" t="s"/>
       <c s="40" r="E18" t="s"/>
-      <c s="40" r="F18" t="s">
-        <v>27</v>
-      </c>
+      <c s="40" r="F18" t="s"/>
       <c s="28" r="G18" t="s"/>
-      <c s="32" r="H18" t="s"/>
+      <c s="40" r="H18" t="s">
+        <v>25</v>
+      </c>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -1637,7 +1635,9 @@
       <c s="40" r="D19" t="s"/>
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
-      <c s="40" r="G19" t="s"/>
+      <c s="40" r="G19" t="s">
+        <v>21</v>
+      </c>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
@@ -1657,7 +1657,7 @@
       <c s="40" r="D20" t="s"/>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
-      <c s="28" r="G20" t="s"/>
+      <c s="40" r="G20" t="s"/>
       <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
@@ -1677,7 +1677,9 @@
       <c s="40" r="D21" t="s"/>
       <c s="40" r="E21" t="s"/>
       <c s="34" r="F21" t="s"/>
-      <c s="40" r="G21" t="s"/>
+      <c s="40" r="G21" t="s">
+        <v>23</v>
+      </c>
       <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
@@ -1694,7 +1696,9 @@
       <c s="2" r="C22" t="n">
         <v>0.8854166666666666</v>
       </c>
-      <c s="40" r="D22" t="s"/>
+      <c s="40" r="D22" t="s">
+        <v>21</v>
+      </c>
       <c s="40" r="E22" t="s"/>
       <c s="40" r="F22" t="s"/>
       <c s="40" r="G22" t="s"/>
@@ -1823,18 +1827,20 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="40" r="D5" t="s"/>
+      <c s="40" r="D5" t="s">
+        <v>29</v>
+      </c>
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
-      <c s="41" r="G5" t="s">
+      <c s="41" r="G5" t="s"/>
+      <c s="40" r="H5" t="s">
         <v>30</v>
       </c>
-      <c s="28" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c s="30" r="J5" t="s">
         <v>31</v>
-      </c>
-      <c s="30" r="J5" t="s">
-        <v>24</v>
       </c>
       <c s="29" r="K5" t="s"/>
       <c s="30" r="L5" t="s"/>
@@ -1849,18 +1855,18 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="28" r="D6" t="s"/>
+      <c s="42" r="D6" t="s">
+        <v>32</v>
+      </c>
       <c s="40" r="E6" t="s"/>
       <c s="40" r="F6" t="s"/>
-      <c s="41" r="G6" t="s">
-        <v>30</v>
-      </c>
+      <c s="41" r="G6" t="s"/>
       <c s="31" r="H6" t="s"/>
       <c s="29" r="I6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="30" r="J6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1875,16 +1881,18 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="28" r="D7" t="s"/>
+      <c s="40" r="D7" t="s">
+        <v>34</v>
+      </c>
       <c s="40" r="E7" t="s"/>
       <c s="40" r="F7" t="s"/>
       <c s="41" r="G7" t="s"/>
-      <c s="36" r="H7" t="s"/>
+      <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c s="30" r="J7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c s="29" r="K7" t="s"/>
       <c s="30" r="L7" t="s"/>
@@ -1901,14 +1909,16 @@
       </c>
       <c s="40" r="D8" t="s"/>
       <c s="40" r="E8" t="s"/>
-      <c s="40" r="F8" t="s"/>
+      <c s="40" r="F8" t="s">
+        <v>33</v>
+      </c>
       <c s="41" r="G8" t="s"/>
       <c s="37" r="H8" t="s"/>
       <c s="29" r="I8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1929,10 +1939,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1947,11 +1957,13 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="37" r="D10" t="s"/>
+      <c s="40" r="D10" t="s">
+        <v>35</v>
+      </c>
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="41" r="G10" t="s"/>
-      <c s="33" r="H10" t="s"/>
+      <c s="40" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
       <c s="29" r="K10" t="s"/>
@@ -1968,16 +1980,12 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="40" r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
-      <c s="41" r="G11" t="s">
-        <v>35</v>
-      </c>
-      <c s="40" r="H11" t="s">
-        <v>30</v>
-      </c>
+      <c s="41" r="G11" t="s"/>
+      <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
       <c s="30" r="J11" t="s"/>
       <c s="29" r="K11" t="s"/>
@@ -1996,7 +2004,7 @@
       <c s="28" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
       <c s="40" r="F12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c s="41" r="G12" t="s"/>
       <c s="40" r="H12" t="s"/>
@@ -2016,9 +2024,7 @@
         <v>0.5798611111111112</v>
       </c>
       <c s="40" r="D13" t="s"/>
-      <c s="40" r="E13" t="s">
-        <v>32</v>
-      </c>
+      <c s="39" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
       <c s="41" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
@@ -2041,7 +2047,7 @@
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
-      <c s="28" r="H14" t="s"/>
+      <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -2058,7 +2064,7 @@
         <v>0.6493055555555556</v>
       </c>
       <c s="40" r="D15" t="s"/>
-      <c s="33" r="E15" t="s"/>
+      <c s="40" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
@@ -2077,17 +2083,11 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="40" r="D16" t="s">
-        <v>31</v>
-      </c>
+      <c s="40" r="D16" t="s"/>
       <c s="28" r="E16" t="s"/>
       <c s="34" r="F16" t="s"/>
-      <c s="40" r="G16" t="s">
-        <v>35</v>
-      </c>
-      <c s="40" r="H16" t="s">
-        <v>33</v>
-      </c>
+      <c s="40" r="G16" t="s"/>
+      <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
       <c s="29" r="K16" t="s"/>
@@ -2107,7 +2107,7 @@
       <c s="28" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="38" r="H17" t="s"/>
+      <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -2147,9 +2147,7 @@
       <c s="28" r="E19" t="s"/>
       <c s="28" r="F19" t="s"/>
       <c s="40" r="G19" t="s"/>
-      <c s="40" r="H19" t="s">
-        <v>31</v>
-      </c>
+      <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
       <c s="29" r="K19" t="s"/>
@@ -2165,10 +2163,12 @@
       <c s="2" r="C20" t="n">
         <v>0.8229166666666666</v>
       </c>
-      <c s="40" r="D20" t="s"/>
+      <c s="40" r="D20" t="s">
+        <v>34</v>
+      </c>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
-      <c s="28" r="G20" t="s"/>
+      <c s="40" r="G20" t="s"/>
       <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
@@ -2454,7 +2454,7 @@
       <c s="2" r="C11" t="n">
         <v>0.5104166666666666</v>
       </c>
-      <c s="32" r="D11" t="s"/>
+      <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
       <c s="38" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
@@ -2497,7 +2497,7 @@
       <c s="40" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
-      <c s="33" r="G13" t="s"/>
+      <c s="40" r="G13" t="s"/>
       <c s="41" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
@@ -2518,7 +2518,7 @@
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
-      <c s="28" r="H14" t="s"/>
+      <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -2535,7 +2535,7 @@
         <v>0.6493055555555556</v>
       </c>
       <c s="40" r="D15" t="s"/>
-      <c s="33" r="E15" t="s"/>
+      <c s="40" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
@@ -2578,7 +2578,7 @@
       <c s="28" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="38" r="H17" t="s"/>
+      <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -2637,7 +2637,7 @@
       <c s="40" r="D20" t="s"/>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
-      <c s="28" r="G20" t="s"/>
+      <c s="40" r="G20" t="s"/>
       <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>
@@ -2847,7 +2847,7 @@
       <c s="40" r="E7" t="s"/>
       <c s="40" r="F7" t="s"/>
       <c s="35" r="G7" t="s"/>
-      <c s="36" r="H7" t="s"/>
+      <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
       <c s="30" r="J7" t="s"/>
       <c s="29" r="K7" t="s"/>
@@ -2907,7 +2907,7 @@
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="40" r="G10" t="s"/>
-      <c s="33" r="H10" t="s"/>
+      <c s="40" r="H10" t="s"/>
       <c s="29" r="I10" t="s"/>
       <c s="30" r="J10" t="s"/>
       <c s="29" r="K10" t="s"/>
@@ -2966,7 +2966,7 @@
       <c s="41" r="D13" t="s"/>
       <c s="39" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
-      <c s="33" r="G13" t="s"/>
+      <c s="40" r="G13" t="s"/>
       <c s="28" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
@@ -2987,7 +2987,7 @@
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
       <c s="32" r="G14" t="s"/>
-      <c s="28" r="H14" t="s"/>
+      <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
       <c s="29" r="K14" t="s"/>
@@ -3004,7 +3004,7 @@
         <v>0.6493055555555556</v>
       </c>
       <c s="40" r="D15" t="s"/>
-      <c s="33" r="E15" t="s"/>
+      <c s="40" r="E15" t="s"/>
       <c s="32" r="F15" t="s"/>
       <c s="28" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
@@ -3047,7 +3047,7 @@
       <c s="28" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
       <c s="28" r="G17" t="s"/>
-      <c s="38" r="H17" t="s"/>
+      <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
       <c s="29" r="K17" t="s"/>
@@ -3106,7 +3106,7 @@
       <c s="40" r="D20" t="s"/>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
-      <c s="28" r="G20" t="s"/>
+      <c s="40" r="G20" t="s"/>
       <c s="40" r="H20" t="s"/>
       <c s="29" r="I20" t="s"/>
       <c s="30" r="J20" t="s"/>

</xml_diff>

<commit_message>
AG Finished: experiment with AG Values to get better solutions
</commit_message>
<xml_diff>
--- a/Proyecto/data/horarioEstudiantes.xlsx
+++ b/Proyecto/data/horarioEstudiantes.xlsx
@@ -59,73 +59,73 @@
     <t>10IE2016</t>
   </si>
   <si>
+    <t>profesor1_apellidoapellido2</t>
+  </si>
+  <si>
+    <t>Receso</t>
+  </si>
+  <si>
+    <t>Periodo Prohibido</t>
+  </si>
+  <si>
+    <t>Periodo Error: Cruzado</t>
+  </si>
+  <si>
+    <t>Periodo Libre</t>
+  </si>
+  <si>
+    <t>20IE2010</t>
+  </si>
+  <si>
+    <t>30IE2010</t>
+  </si>
+  <si>
+    <t>Profesor4_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>10IE2010</t>
+  </si>
+  <si>
+    <t>20IE2009</t>
+  </si>
+  <si>
+    <t>MaurucioRodrigo_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>10IE2011</t>
+  </si>
+  <si>
+    <t>30IE2009</t>
+  </si>
+  <si>
     <t>DiegoPablo_RegaladoSamayoa</t>
   </si>
   <si>
-    <t>Receso</t>
-  </si>
-  <si>
-    <t>Periodo Prohibido</t>
-  </si>
-  <si>
-    <t>Periodo Error: Cruzado</t>
-  </si>
-  <si>
-    <t>Periodo Libre</t>
-  </si>
-  <si>
-    <t>30IE2010</t>
-  </si>
-  <si>
-    <t>30IE2009</t>
-  </si>
-  <si>
     <t>10IE2008</t>
   </si>
   <si>
-    <t>20IE2010</t>
-  </si>
-  <si>
-    <t>Profesor4SegundoN_Apellido1Apellido2</t>
-  </si>
-  <si>
-    <t>20IE2009</t>
-  </si>
-  <si>
-    <t>Profesor5segundoN5_Apellido1Apellido2</t>
-  </si>
-  <si>
-    <t>10IE2010</t>
-  </si>
-  <si>
-    <t>10IE2011</t>
-  </si>
-  <si>
     <t>10IE2009</t>
   </si>
   <si>
-    <t>Miguelnose_apellidoapellido2</t>
+    <t>10IE2010, 10IE2009</t>
   </si>
   <si>
     <t>10IE3028</t>
   </si>
   <si>
+    <t>10IE3048</t>
+  </si>
+  <si>
+    <t>profesor5_Apellido1Apellido2</t>
+  </si>
+  <si>
+    <t>10IE2013</t>
+  </si>
+  <si>
+    <t>10IE3049</t>
+  </si>
+  <si>
     <t>20IE3028</t>
-  </si>
-  <si>
-    <t>MaurucioRodrigo_Apellido1Sepa</t>
-  </si>
-  <si>
-    <t>10IE3028, 10IE3049, 20IE3028</t>
-  </si>
-  <si>
-    <t>10IE3048</t>
-  </si>
-  <si>
-    <t>10IE3049</t>
-  </si>
-  <si>
-    <t>10IE2013</t>
   </si>
 </sst>
 </file>
@@ -809,10 +809,10 @@
       <c s="40" r="D5" t="s"/>
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
-      <c s="28" r="G5" t="s"/>
-      <c s="40" r="H5" t="s">
+      <c s="40" r="G5" t="s">
         <v>12</v>
       </c>
+      <c s="40" r="H5" t="s"/>
       <c s="29" r="I5" t="s">
         <v>12</v>
       </c>
@@ -832,13 +832,13 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="28" r="D6" t="s"/>
+      <c s="40" r="D6" t="s"/>
       <c s="40" r="E6" t="s"/>
-      <c s="40" r="F6" t="s">
+      <c s="40" r="F6" t="s"/>
+      <c s="40" r="G6" t="s">
         <v>12</v>
       </c>
-      <c s="40" r="G6" t="s"/>
-      <c s="31" r="H6" t="s"/>
+      <c s="40" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
       <c s="30" r="J6" t="s"/>
       <c s="29" r="K6" t="s"/>
@@ -854,12 +854,12 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="28" r="D7" t="s"/>
+      <c s="40" r="D7" t="s"/>
       <c s="40" r="E7" t="s"/>
-      <c s="40" r="F7" t="s">
+      <c s="40" r="F7" t="s"/>
+      <c s="40" r="G7" t="s">
         <v>12</v>
       </c>
-      <c s="35" r="G7" t="s"/>
       <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
       <c s="30" r="J7" t="s"/>
@@ -880,7 +880,7 @@
       <c s="40" r="E8" t="s"/>
       <c s="40" r="F8" t="s"/>
       <c s="40" r="G8" t="s"/>
-      <c s="37" r="H8" t="s"/>
+      <c s="40" r="H8" t="s"/>
       <c s="29" r="I8" t="s"/>
       <c s="30" r="J8" t="s"/>
       <c s="29" r="K8" t="s"/>
@@ -916,7 +916,7 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="37" r="D10" t="s"/>
+      <c s="40" r="D10" t="s"/>
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="40" r="G10" t="s"/>
@@ -938,7 +938,7 @@
       </c>
       <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
-      <c s="38" r="F11" t="s"/>
+      <c s="40" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
       <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
@@ -956,10 +956,10 @@
       <c s="2" r="C12" t="n">
         <v>0.5451388888888888</v>
       </c>
-      <c s="28" r="D12" t="s"/>
+      <c s="40" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
       <c s="40" r="F12" t="s"/>
-      <c s="32" r="G12" t="s"/>
+      <c s="40" r="G12" t="s"/>
       <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
@@ -977,10 +977,10 @@
         <v>0.5798611111111112</v>
       </c>
       <c s="40" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
+      <c s="40" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
       <c s="40" r="G13" t="s"/>
-      <c s="28" r="H13" t="s"/>
+      <c s="40" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
       <c s="29" r="K13" t="s"/>
@@ -999,7 +999,7 @@
       <c s="40" r="D14" t="s"/>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="G14" t="s"/>
       <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -1018,8 +1018,8 @@
       </c>
       <c s="40" r="D15" t="s"/>
       <c s="40" r="E15" t="s"/>
-      <c s="32" r="F15" t="s"/>
-      <c s="28" r="G15" t="s"/>
+      <c s="40" r="F15" t="s"/>
+      <c s="40" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
@@ -1037,8 +1037,8 @@
         <v>0.6840277777777778</v>
       </c>
       <c s="40" r="D16" t="s"/>
-      <c s="28" r="E16" t="s"/>
-      <c s="34" r="F16" t="s"/>
+      <c s="40" r="E16" t="s"/>
+      <c s="40" r="F16" t="s"/>
       <c s="40" r="G16" t="s"/>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
@@ -1057,9 +1057,9 @@
         <v>0.71875</v>
       </c>
       <c s="40" r="D17" t="s"/>
-      <c s="28" r="E17" t="s"/>
+      <c s="40" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
-      <c s="28" r="G17" t="s"/>
+      <c s="40" r="G17" t="s"/>
       <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
@@ -1076,11 +1076,11 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="28" r="D18" t="s"/>
+      <c s="40" r="D18" t="s"/>
       <c s="40" r="E18" t="s"/>
       <c s="40" r="F18" t="s"/>
-      <c s="28" r="G18" t="s"/>
-      <c s="32" r="H18" t="s"/>
+      <c s="40" r="G18" t="s"/>
+      <c s="40" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -1097,8 +1097,8 @@
         <v>0.7881944444444444</v>
       </c>
       <c s="40" r="D19" t="s"/>
-      <c s="28" r="E19" t="s"/>
-      <c s="28" r="F19" t="s"/>
+      <c s="40" r="E19" t="s"/>
+      <c s="40" r="F19" t="s"/>
       <c s="40" r="G19" t="s"/>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c s="40" r="D21" t="s"/>
       <c s="40" r="E21" t="s"/>
-      <c s="34" r="F21" t="s"/>
+      <c s="40" r="F21" t="s"/>
       <c s="40" r="G21" t="s"/>
       <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
@@ -1289,19 +1289,17 @@
       <c s="40" r="D5" t="s">
         <v>18</v>
       </c>
-      <c s="40" r="E5" t="s">
+      <c s="40" r="E5" t="s"/>
+      <c s="41" r="F5" t="s"/>
+      <c s="40" r="G5" t="s"/>
+      <c s="40" r="H5" t="s">
         <v>19</v>
       </c>
-      <c s="41" r="F5" t="s"/>
-      <c s="40" r="G5" t="s">
+      <c s="29" r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c s="30" r="J5" t="s">
         <v>20</v>
-      </c>
-      <c s="28" r="H5" t="s"/>
-      <c s="29" r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c s="30" r="J5" t="s">
-        <v>22</v>
       </c>
       <c s="29" r="K5" t="s"/>
       <c s="30" r="L5" t="s"/>
@@ -1316,22 +1314,20 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="40" r="D6" t="s">
-        <v>18</v>
-      </c>
+      <c s="40" r="D6" t="s"/>
       <c s="40" r="E6" t="s"/>
-      <c s="41" r="F6" t="s"/>
-      <c s="40" r="G6" t="s">
+      <c s="41" r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c s="40" r="G6" t="s"/>
+      <c s="40" r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c s="29" r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c s="30" r="J6" t="s">
         <v>23</v>
-      </c>
-      <c s="40" r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c s="29" r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c s="30" r="J6" t="s">
-        <v>22</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1351,15 +1347,15 @@
       </c>
       <c s="40" r="E7" t="s"/>
       <c s="41" r="F7" t="s"/>
-      <c s="35" r="G7" t="s"/>
+      <c s="40" r="G7" t="s"/>
       <c s="40" r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c s="29" r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c s="30" r="J7" t="s">
         <v>20</v>
-      </c>
-      <c s="29" r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c s="30" r="J7" t="s">
-        <v>24</v>
       </c>
       <c s="29" r="K7" t="s"/>
       <c s="30" r="L7" t="s"/>
@@ -1378,14 +1374,12 @@
       <c s="40" r="E8" t="s"/>
       <c s="41" r="F8" t="s"/>
       <c s="40" r="G8" t="s"/>
-      <c s="40" r="H8" t="s">
-        <v>25</v>
-      </c>
+      <c s="40" r="H8" t="s"/>
       <c s="29" r="I8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1406,10 +1400,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1424,20 +1418,18 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="37" r="D10" t="s"/>
-      <c s="40" r="E10" t="s">
-        <v>27</v>
-      </c>
+      <c s="40" r="D10" t="s"/>
+      <c s="40" r="E10" t="s"/>
       <c s="41" r="F10" t="s"/>
       <c s="40" r="G10" t="s"/>
       <c s="40" r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c s="29" r="I10" t="s">
         <v>25</v>
       </c>
-      <c s="29" r="I10" t="s">
-        <v>19</v>
-      </c>
       <c s="30" r="J10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c s="29" r="K10" t="s"/>
       <c s="30" r="L10" t="s"/>
@@ -1453,17 +1445,17 @@
         <v>0.5104166666666666</v>
       </c>
       <c s="40" r="D11" t="s"/>
-      <c s="40" r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c s="41" r="F11" t="s"/>
+      <c s="40" r="E11" t="s"/>
+      <c s="41" r="F11" t="s">
+        <v>21</v>
+      </c>
       <c s="40" r="G11" t="s"/>
       <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c s="30" r="J11" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c s="29" r="K11" t="s"/>
       <c s="30" r="L11" t="s"/>
@@ -1478,16 +1470,16 @@
       <c s="2" r="C12" t="n">
         <v>0.5451388888888888</v>
       </c>
-      <c s="28" r="D12" t="s"/>
+      <c s="40" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
       <c s="41" r="F12" t="s"/>
-      <c s="32" r="G12" t="s"/>
+      <c s="40" r="G12" t="s"/>
       <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="30" r="J12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c s="29" r="K12" t="s"/>
       <c s="30" r="L12" t="s"/>
@@ -1502,11 +1494,13 @@
       <c s="2" r="C13" t="n">
         <v>0.5798611111111112</v>
       </c>
-      <c s="40" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
+      <c s="40" r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c s="40" r="E13" t="s"/>
       <c s="41" r="F13" t="s"/>
       <c s="40" r="G13" t="s"/>
-      <c s="28" r="H13" t="s"/>
+      <c s="40" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
       <c s="29" r="K13" t="s"/>
@@ -1522,10 +1516,12 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="40" r="D14" t="s"/>
+      <c s="40" r="D14" t="s">
+        <v>27</v>
+      </c>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="G14" t="s"/>
       <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -1542,13 +1538,15 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="40" r="D15" t="s"/>
-      <c s="40" r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c s="32" r="F15" t="s"/>
-      <c s="28" r="G15" t="s"/>
-      <c s="40" r="H15" t="s"/>
+      <c s="40" r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c s="40" r="E15" t="s"/>
+      <c s="40" r="F15" t="s"/>
+      <c s="40" r="G15" t="s"/>
+      <c s="40" r="H15" t="s">
+        <v>24</v>
+      </c>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
       <c s="29" r="K15" t="s"/>
@@ -1565,13 +1563,13 @@
         <v>0.6840277777777778</v>
       </c>
       <c s="40" r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c s="28" r="E16" t="s"/>
-      <c s="34" r="F16" t="s"/>
-      <c s="40" r="G16" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c s="40" r="E16" t="s"/>
+      <c s="40" r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c s="40" r="G16" t="s"/>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
       <c s="30" r="J16" t="s"/>
@@ -1588,12 +1586,12 @@
       <c s="2" r="C17" t="n">
         <v>0.71875</v>
       </c>
-      <c s="40" r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c s="28" r="E17" t="s"/>
-      <c s="40" r="F17" t="s"/>
-      <c s="28" r="G17" t="s"/>
+      <c s="40" r="D17" t="s"/>
+      <c s="40" r="E17" t="s"/>
+      <c s="42" r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c s="40" r="G17" t="s"/>
       <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
@@ -1610,13 +1608,13 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="28" r="D18" t="s"/>
+      <c s="40" r="D18" t="s">
+        <v>27</v>
+      </c>
       <c s="40" r="E18" t="s"/>
       <c s="40" r="F18" t="s"/>
-      <c s="28" r="G18" t="s"/>
-      <c s="40" r="H18" t="s">
-        <v>25</v>
-      </c>
+      <c s="40" r="G18" t="s"/>
+      <c s="40" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -1633,11 +1631,9 @@
         <v>0.7881944444444444</v>
       </c>
       <c s="40" r="D19" t="s"/>
-      <c s="28" r="E19" t="s"/>
-      <c s="28" r="F19" t="s"/>
-      <c s="40" r="G19" t="s">
-        <v>21</v>
-      </c>
+      <c s="40" r="E19" t="s"/>
+      <c s="40" r="F19" t="s"/>
+      <c s="40" r="G19" t="s"/>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
       <c s="30" r="J19" t="s"/>
@@ -1676,11 +1672,11 @@
       </c>
       <c s="40" r="D21" t="s"/>
       <c s="40" r="E21" t="s"/>
-      <c s="34" r="F21" t="s"/>
-      <c s="40" r="G21" t="s">
-        <v>23</v>
-      </c>
-      <c s="40" r="H21" t="s"/>
+      <c s="40" r="F21" t="s"/>
+      <c s="40" r="G21" t="s"/>
+      <c s="40" r="H21" t="s">
+        <v>25</v>
+      </c>
       <c s="29" r="I21" t="s"/>
       <c s="30" r="J21" t="s"/>
       <c s="29" r="K21" t="s"/>
@@ -1697,12 +1693,14 @@
         <v>0.8854166666666666</v>
       </c>
       <c s="40" r="D22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c s="40" r="E22" t="s"/>
       <c s="40" r="F22" t="s"/>
       <c s="40" r="G22" t="s"/>
-      <c s="40" r="H22" t="s"/>
+      <c s="40" r="H22" t="s">
+        <v>25</v>
+      </c>
       <c s="29" r="I22" t="s"/>
       <c s="30" r="J22" t="s"/>
       <c s="29" r="K22" t="s"/>
@@ -1827,20 +1825,16 @@
       <c s="2" r="C5" t="n">
         <v>0.3229166666666667</v>
       </c>
-      <c s="40" r="D5" t="s">
-        <v>29</v>
-      </c>
+      <c s="40" r="D5" t="s"/>
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
       <c s="41" r="G5" t="s"/>
-      <c s="40" r="H5" t="s">
+      <c s="40" r="H5" t="s"/>
+      <c s="29" r="I5" t="s">
         <v>30</v>
       </c>
-      <c s="29" r="I5" t="s">
-        <v>29</v>
-      </c>
       <c s="30" r="J5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c s="29" r="K5" t="s"/>
       <c s="30" r="L5" t="s"/>
@@ -1855,18 +1849,16 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="42" r="D6" t="s">
-        <v>32</v>
-      </c>
+      <c s="40" r="D6" t="s"/>
       <c s="40" r="E6" t="s"/>
       <c s="40" r="F6" t="s"/>
       <c s="41" r="G6" t="s"/>
-      <c s="31" r="H6" t="s"/>
+      <c s="40" r="H6" t="s"/>
       <c s="29" r="I6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c s="30" r="J6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c s="29" r="K6" t="s"/>
       <c s="30" r="L6" t="s"/>
@@ -1881,18 +1873,16 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="40" r="D7" t="s">
-        <v>34</v>
-      </c>
+      <c s="40" r="D7" t="s"/>
       <c s="40" r="E7" t="s"/>
       <c s="40" r="F7" t="s"/>
       <c s="41" r="G7" t="s"/>
       <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c s="30" r="J7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c s="29" r="K7" t="s"/>
       <c s="30" r="L7" t="s"/>
@@ -1909,16 +1899,14 @@
       </c>
       <c s="40" r="D8" t="s"/>
       <c s="40" r="E8" t="s"/>
-      <c s="40" r="F8" t="s">
-        <v>33</v>
-      </c>
+      <c s="40" r="F8" t="s"/>
       <c s="41" r="G8" t="s"/>
-      <c s="37" r="H8" t="s"/>
+      <c s="40" r="H8" t="s"/>
       <c s="29" r="I8" t="s">
         <v>34</v>
       </c>
       <c s="30" r="J8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c s="29" r="K8" t="s"/>
       <c s="30" r="L8" t="s"/>
@@ -1939,10 +1927,10 @@
       <c s="33" r="G9" t="s"/>
       <c s="28" r="H9" t="s"/>
       <c s="29" r="I9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c s="30" r="J9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c s="29" r="K9" t="s"/>
       <c s="30" r="L9" t="s"/>
@@ -1957,9 +1945,7 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="40" r="D10" t="s">
-        <v>35</v>
-      </c>
+      <c s="40" r="D10" t="s"/>
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="41" r="G10" t="s"/>
@@ -1979,11 +1965,9 @@
       <c s="2" r="C11" t="n">
         <v>0.5104166666666666</v>
       </c>
-      <c s="40" r="D11" t="s">
-        <v>35</v>
-      </c>
+      <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
-      <c s="38" r="F11" t="s"/>
+      <c s="40" r="F11" t="s"/>
       <c s="41" r="G11" t="s"/>
       <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
@@ -2001,11 +1985,9 @@
       <c s="2" r="C12" t="n">
         <v>0.5451388888888888</v>
       </c>
-      <c s="28" r="D12" t="s"/>
+      <c s="40" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
-      <c s="40" r="F12" t="s">
-        <v>35</v>
-      </c>
+      <c s="40" r="F12" t="s"/>
       <c s="41" r="G12" t="s"/>
       <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
@@ -2024,10 +2006,10 @@
         <v>0.5798611111111112</v>
       </c>
       <c s="40" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
+      <c s="40" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
       <c s="41" r="G13" t="s"/>
-      <c s="28" r="H13" t="s"/>
+      <c s="40" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
       <c s="29" r="K13" t="s"/>
@@ -2043,10 +2025,12 @@
       <c s="2" r="C14" t="n">
         <v>0.6145833333333334</v>
       </c>
-      <c s="40" r="D14" t="s"/>
+      <c s="40" r="D14" t="s">
+        <v>34</v>
+      </c>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="G14" t="s"/>
       <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -2063,10 +2047,12 @@
       <c s="2" r="C15" t="n">
         <v>0.6493055555555556</v>
       </c>
-      <c s="40" r="D15" t="s"/>
+      <c s="40" r="D15" t="s">
+        <v>30</v>
+      </c>
       <c s="40" r="E15" t="s"/>
-      <c s="32" r="F15" t="s"/>
-      <c s="28" r="G15" t="s"/>
+      <c s="40" r="F15" t="s"/>
+      <c s="40" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
@@ -2083,9 +2069,13 @@
       <c s="2" r="C16" t="n">
         <v>0.6840277777777778</v>
       </c>
-      <c s="40" r="D16" t="s"/>
-      <c s="28" r="E16" t="s"/>
-      <c s="34" r="F16" t="s"/>
+      <c s="40" r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c s="40" r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c s="40" r="F16" t="s"/>
       <c s="40" r="G16" t="s"/>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
@@ -2104,9 +2094,11 @@
         <v>0.71875</v>
       </c>
       <c s="40" r="D17" t="s"/>
-      <c s="28" r="E17" t="s"/>
+      <c s="40" r="E17" t="s">
+        <v>33</v>
+      </c>
       <c s="40" r="F17" t="s"/>
-      <c s="28" r="G17" t="s"/>
+      <c s="40" r="G17" t="s"/>
       <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
@@ -2123,11 +2115,13 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="28" r="D18" t="s"/>
+      <c s="40" r="D18" t="s">
+        <v>34</v>
+      </c>
       <c s="40" r="E18" t="s"/>
       <c s="40" r="F18" t="s"/>
-      <c s="28" r="G18" t="s"/>
-      <c s="32" r="H18" t="s"/>
+      <c s="40" r="G18" t="s"/>
+      <c s="40" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -2144,8 +2138,10 @@
         <v>0.7881944444444444</v>
       </c>
       <c s="40" r="D19" t="s"/>
-      <c s="28" r="E19" t="s"/>
-      <c s="28" r="F19" t="s"/>
+      <c s="40" r="E19" t="s"/>
+      <c s="40" r="F19" t="s">
+        <v>35</v>
+      </c>
       <c s="40" r="G19" t="s"/>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
@@ -2164,7 +2160,7 @@
         <v>0.8229166666666666</v>
       </c>
       <c s="40" r="D20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c s="40" r="E20" t="s"/>
       <c s="40" r="F20" t="s"/>
@@ -2185,9 +2181,11 @@
       <c s="2" r="C21" t="n">
         <v>0.8576388888888888</v>
       </c>
-      <c s="40" r="D21" t="s"/>
+      <c s="40" r="D21" t="s">
+        <v>34</v>
+      </c>
       <c s="40" r="E21" t="s"/>
-      <c s="34" r="F21" t="s"/>
+      <c s="40" r="F21" t="s"/>
       <c s="40" r="G21" t="s"/>
       <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
@@ -2206,8 +2204,12 @@
         <v>0.8854166666666666</v>
       </c>
       <c s="40" r="D22" t="s"/>
-      <c s="40" r="E22" t="s"/>
-      <c s="40" r="F22" t="s"/>
+      <c s="40" r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c s="40" r="F22" t="s">
+        <v>35</v>
+      </c>
       <c s="40" r="G22" t="s"/>
       <c s="40" r="H22" t="s"/>
       <c s="29" r="I22" t="s"/>
@@ -2337,7 +2339,7 @@
       <c s="40" r="D5" t="s"/>
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
-      <c s="28" r="G5" t="s"/>
+      <c s="40" r="G5" t="s"/>
       <c s="41" r="H5" t="s"/>
       <c s="29" r="I5" t="s"/>
       <c s="30" r="J5" t="s"/>
@@ -2354,7 +2356,7 @@
       <c s="2" r="C6" t="n">
         <v>0.3576388888888889</v>
       </c>
-      <c s="28" r="D6" t="s"/>
+      <c s="40" r="D6" t="s"/>
       <c s="40" r="E6" t="s"/>
       <c s="40" r="F6" t="s"/>
       <c s="40" r="G6" t="s"/>
@@ -2374,10 +2376,10 @@
       <c s="2" r="C7" t="n">
         <v>0.3923611111111111</v>
       </c>
-      <c s="28" r="D7" t="s"/>
+      <c s="40" r="D7" t="s"/>
       <c s="40" r="E7" t="s"/>
       <c s="40" r="F7" t="s"/>
-      <c s="35" r="G7" t="s"/>
+      <c s="40" r="G7" t="s"/>
       <c s="41" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
       <c s="30" r="J7" t="s"/>
@@ -2434,7 +2436,7 @@
       <c s="2" r="C10" t="n">
         <v>0.4756944444444444</v>
       </c>
-      <c s="37" r="D10" t="s"/>
+      <c s="40" r="D10" t="s"/>
       <c s="40" r="E10" t="s"/>
       <c s="40" r="F10" t="s"/>
       <c s="40" r="G10" t="s"/>
@@ -2456,7 +2458,7 @@
       </c>
       <c s="40" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
-      <c s="38" r="F11" t="s"/>
+      <c s="40" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
       <c s="41" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
@@ -2474,10 +2476,10 @@
       <c s="2" r="C12" t="n">
         <v>0.5451388888888888</v>
       </c>
-      <c s="28" r="D12" t="s"/>
+      <c s="40" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
       <c s="40" r="F12" t="s"/>
-      <c s="32" r="G12" t="s"/>
+      <c s="40" r="G12" t="s"/>
       <c s="41" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
@@ -2495,7 +2497,7 @@
         <v>0.5798611111111112</v>
       </c>
       <c s="40" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
+      <c s="40" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
       <c s="40" r="G13" t="s"/>
       <c s="41" r="H13" t="s"/>
@@ -2517,7 +2519,7 @@
       <c s="40" r="D14" t="s"/>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="G14" t="s"/>
       <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -2536,8 +2538,8 @@
       </c>
       <c s="40" r="D15" t="s"/>
       <c s="40" r="E15" t="s"/>
-      <c s="32" r="F15" t="s"/>
-      <c s="28" r="G15" t="s"/>
+      <c s="40" r="F15" t="s"/>
+      <c s="40" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
@@ -2555,8 +2557,8 @@
         <v>0.6840277777777778</v>
       </c>
       <c s="40" r="D16" t="s"/>
-      <c s="28" r="E16" t="s"/>
-      <c s="34" r="F16" t="s"/>
+      <c s="40" r="E16" t="s"/>
+      <c s="40" r="F16" t="s"/>
       <c s="40" r="G16" t="s"/>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
@@ -2575,9 +2577,9 @@
         <v>0.71875</v>
       </c>
       <c s="40" r="D17" t="s"/>
-      <c s="28" r="E17" t="s"/>
+      <c s="40" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
-      <c s="28" r="G17" t="s"/>
+      <c s="40" r="G17" t="s"/>
       <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
@@ -2594,11 +2596,11 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="28" r="D18" t="s"/>
+      <c s="40" r="D18" t="s"/>
       <c s="40" r="E18" t="s"/>
       <c s="40" r="F18" t="s"/>
-      <c s="28" r="G18" t="s"/>
-      <c s="32" r="H18" t="s"/>
+      <c s="40" r="G18" t="s"/>
+      <c s="40" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -2615,8 +2617,8 @@
         <v>0.7881944444444444</v>
       </c>
       <c s="40" r="D19" t="s"/>
-      <c s="28" r="E19" t="s"/>
-      <c s="28" r="F19" t="s"/>
+      <c s="40" r="E19" t="s"/>
+      <c s="40" r="F19" t="s"/>
       <c s="40" r="G19" t="s"/>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
@@ -2656,7 +2658,7 @@
       </c>
       <c s="40" r="D21" t="s"/>
       <c s="40" r="E21" t="s"/>
-      <c s="34" r="F21" t="s"/>
+      <c s="40" r="F21" t="s"/>
       <c s="40" r="G21" t="s"/>
       <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>
@@ -2806,8 +2808,8 @@
       <c s="41" r="D5" t="s"/>
       <c s="40" r="E5" t="s"/>
       <c s="40" r="F5" t="s"/>
-      <c s="28" r="G5" t="s"/>
-      <c s="28" r="H5" t="s"/>
+      <c s="40" r="G5" t="s"/>
+      <c s="40" r="H5" t="s"/>
       <c s="29" r="I5" t="s"/>
       <c s="30" r="J5" t="s"/>
       <c s="29" r="K5" t="s"/>
@@ -2827,7 +2829,7 @@
       <c s="40" r="E6" t="s"/>
       <c s="40" r="F6" t="s"/>
       <c s="40" r="G6" t="s"/>
-      <c s="31" r="H6" t="s"/>
+      <c s="40" r="H6" t="s"/>
       <c s="29" r="I6" t="s"/>
       <c s="30" r="J6" t="s"/>
       <c s="29" r="K6" t="s"/>
@@ -2846,7 +2848,7 @@
       <c s="41" r="D7" t="s"/>
       <c s="40" r="E7" t="s"/>
       <c s="40" r="F7" t="s"/>
-      <c s="35" r="G7" t="s"/>
+      <c s="40" r="G7" t="s"/>
       <c s="40" r="H7" t="s"/>
       <c s="29" r="I7" t="s"/>
       <c s="30" r="J7" t="s"/>
@@ -2867,7 +2869,7 @@
       <c s="40" r="E8" t="s"/>
       <c s="40" r="F8" t="s"/>
       <c s="40" r="G8" t="s"/>
-      <c s="37" r="H8" t="s"/>
+      <c s="40" r="H8" t="s"/>
       <c s="29" r="I8" t="s"/>
       <c s="30" r="J8" t="s"/>
       <c s="29" r="K8" t="s"/>
@@ -2925,7 +2927,7 @@
       </c>
       <c s="41" r="D11" t="s"/>
       <c s="40" r="E11" t="s"/>
-      <c s="38" r="F11" t="s"/>
+      <c s="40" r="F11" t="s"/>
       <c s="40" r="G11" t="s"/>
       <c s="40" r="H11" t="s"/>
       <c s="29" r="I11" t="s"/>
@@ -2946,7 +2948,7 @@
       <c s="41" r="D12" t="s"/>
       <c s="40" r="E12" t="s"/>
       <c s="40" r="F12" t="s"/>
-      <c s="32" r="G12" t="s"/>
+      <c s="40" r="G12" t="s"/>
       <c s="40" r="H12" t="s"/>
       <c s="29" r="I12" t="s"/>
       <c s="30" r="J12" t="s"/>
@@ -2964,10 +2966,10 @@
         <v>0.5798611111111112</v>
       </c>
       <c s="41" r="D13" t="s"/>
-      <c s="39" r="E13" t="s"/>
+      <c s="40" r="E13" t="s"/>
       <c s="40" r="F13" t="s"/>
       <c s="40" r="G13" t="s"/>
-      <c s="28" r="H13" t="s"/>
+      <c s="40" r="H13" t="s"/>
       <c s="29" r="I13" t="s"/>
       <c s="30" r="J13" t="s"/>
       <c s="29" r="K13" t="s"/>
@@ -2986,7 +2988,7 @@
       <c s="40" r="D14" t="s"/>
       <c s="40" r="E14" t="s"/>
       <c s="40" r="F14" t="s"/>
-      <c s="32" r="G14" t="s"/>
+      <c s="40" r="G14" t="s"/>
       <c s="40" r="H14" t="s"/>
       <c s="29" r="I14" t="s"/>
       <c s="30" r="J14" t="s"/>
@@ -3005,8 +3007,8 @@
       </c>
       <c s="40" r="D15" t="s"/>
       <c s="40" r="E15" t="s"/>
-      <c s="32" r="F15" t="s"/>
-      <c s="28" r="G15" t="s"/>
+      <c s="40" r="F15" t="s"/>
+      <c s="40" r="G15" t="s"/>
       <c s="40" r="H15" t="s"/>
       <c s="29" r="I15" t="s"/>
       <c s="30" r="J15" t="s"/>
@@ -3024,8 +3026,8 @@
         <v>0.6840277777777778</v>
       </c>
       <c s="40" r="D16" t="s"/>
-      <c s="28" r="E16" t="s"/>
-      <c s="34" r="F16" t="s"/>
+      <c s="40" r="E16" t="s"/>
+      <c s="40" r="F16" t="s"/>
       <c s="40" r="G16" t="s"/>
       <c s="40" r="H16" t="s"/>
       <c s="29" r="I16" t="s"/>
@@ -3044,9 +3046,9 @@
         <v>0.71875</v>
       </c>
       <c s="40" r="D17" t="s"/>
-      <c s="28" r="E17" t="s"/>
+      <c s="40" r="E17" t="s"/>
       <c s="40" r="F17" t="s"/>
-      <c s="28" r="G17" t="s"/>
+      <c s="40" r="G17" t="s"/>
       <c s="40" r="H17" t="s"/>
       <c s="29" r="I17" t="s"/>
       <c s="30" r="J17" t="s"/>
@@ -3063,11 +3065,11 @@
       <c s="2" r="C18" t="n">
         <v>0.7534722222222222</v>
       </c>
-      <c s="28" r="D18" t="s"/>
+      <c s="40" r="D18" t="s"/>
       <c s="40" r="E18" t="s"/>
       <c s="40" r="F18" t="s"/>
-      <c s="28" r="G18" t="s"/>
-      <c s="32" r="H18" t="s"/>
+      <c s="40" r="G18" t="s"/>
+      <c s="40" r="H18" t="s"/>
       <c s="29" r="I18" t="s"/>
       <c s="30" r="J18" t="s"/>
       <c s="29" r="K18" t="s"/>
@@ -3084,8 +3086,8 @@
         <v>0.7881944444444444</v>
       </c>
       <c s="40" r="D19" t="s"/>
-      <c s="28" r="E19" t="s"/>
-      <c s="28" r="F19" t="s"/>
+      <c s="40" r="E19" t="s"/>
+      <c s="40" r="F19" t="s"/>
       <c s="40" r="G19" t="s"/>
       <c s="40" r="H19" t="s"/>
       <c s="29" r="I19" t="s"/>
@@ -3125,7 +3127,7 @@
       </c>
       <c s="40" r="D21" t="s"/>
       <c s="40" r="E21" t="s"/>
-      <c s="34" r="F21" t="s"/>
+      <c s="40" r="F21" t="s"/>
       <c s="40" r="G21" t="s"/>
       <c s="40" r="H21" t="s"/>
       <c s="29" r="I21" t="s"/>

</xml_diff>